<commit_message>
edited table to fix dates and YSI comment under IEC Run #12
</commit_message>
<xml_diff>
--- a/data/CruiseInfoTable2025.xlsx
+++ b/data/CruiseInfoTable2025.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\Projects\2025 Hypoxia Summary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\Projects\2025 Hypoxia Summary\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0BD068-E511-4FA9-8BCD-A24A74E17E51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D492E9C8-48C9-48F1-A7B2-AFFCBCD030B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="66">
   <si>
     <t>Cruise</t>
   </si>
@@ -160,12 +160,90 @@
   </si>
   <si>
     <t>E1</t>
+  </si>
+  <si>
+    <t>6/2/25</t>
+  </si>
+  <si>
+    <t>6/4/25</t>
+  </si>
+  <si>
+    <t>6/18/25</t>
+  </si>
+  <si>
+    <t>6/17/25</t>
+  </si>
+  <si>
+    <t>6/24/25</t>
+  </si>
+  <si>
+    <t>7/2/25</t>
+  </si>
+  <si>
+    <t>6/30/25</t>
+  </si>
+  <si>
+    <t>7/1/25</t>
+  </si>
+  <si>
+    <t>7/8/25</t>
+  </si>
+  <si>
+    <t>7/14/25</t>
+  </si>
+  <si>
+    <t>7/16/25</t>
+  </si>
+  <si>
+    <t>7/18/25</t>
+  </si>
+  <si>
+    <t>7/24/25</t>
+  </si>
+  <si>
+    <t>7/29/25</t>
+  </si>
+  <si>
+    <t>7/31/25</t>
+  </si>
+  <si>
+    <t>8/5/25</t>
+  </si>
+  <si>
+    <t>8/12/25</t>
+  </si>
+  <si>
+    <t>8/11/25</t>
+  </si>
+  <si>
+    <t>8/13/25</t>
+  </si>
+  <si>
+    <t>8/19/25</t>
+  </si>
+  <si>
+    <t>8/26/25</t>
+  </si>
+  <si>
+    <t>8/25/25</t>
+  </si>
+  <si>
+    <t>8/28/25</t>
+  </si>
+  <si>
+    <t>9/2/25</t>
+  </si>
+  <si>
+    <t>9/18/2025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="m/d/yy;@"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -307,7 +385,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -351,6 +429,28 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -631,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection sqref="A1:H22"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -652,7 +752,7 @@
     <col min="16" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -678,15 +778,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="7">
-        <v>45810</v>
-      </c>
-      <c r="C2" s="8">
-        <v>45812</v>
+      <c r="B2" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>42</v>
       </c>
       <c r="D2" s="9">
         <v>17</v>
@@ -703,16 +803,18 @@
       <c r="H2" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+    </row>
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="7">
-        <v>45825</v>
-      </c>
-      <c r="C3" s="8">
-        <v>45826</v>
+      <c r="B3" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>43</v>
       </c>
       <c r="D3" s="9">
         <v>30</v>
@@ -729,16 +831,18 @@
       <c r="H3" s="9" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="7">
-        <v>45832</v>
-      </c>
-      <c r="C4" s="8">
-        <v>45832</v>
+      <c r="B4" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>45</v>
       </c>
       <c r="D4" s="9">
         <v>23</v>
@@ -755,16 +859,18 @@
       <c r="H4" s="6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+    </row>
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="7">
-        <v>45838</v>
-      </c>
-      <c r="C5" s="8">
-        <v>45840</v>
+      <c r="B5" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>46</v>
       </c>
       <c r="D5" s="9">
         <v>40</v>
@@ -781,16 +887,18 @@
       <c r="H5" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+    </row>
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="7">
-        <v>45839</v>
-      </c>
-      <c r="C6" s="8">
-        <v>45839</v>
+      <c r="B6" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>48</v>
       </c>
       <c r="D6" s="9">
         <v>24</v>
@@ -807,16 +915,18 @@
       <c r="H6" s="9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+    </row>
+    <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="7">
-        <v>45846</v>
-      </c>
-      <c r="C7" s="8">
-        <v>45846</v>
+      <c r="B7" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>49</v>
       </c>
       <c r="D7" s="9">
         <v>24</v>
@@ -833,16 +943,18 @@
       <c r="H7" s="9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+    </row>
+    <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="7">
-        <v>45852</v>
-      </c>
-      <c r="C8" s="8">
-        <v>45854</v>
+      <c r="B8" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>51</v>
       </c>
       <c r="D8" s="9">
         <v>39</v>
@@ -859,16 +971,18 @@
       <c r="H8" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+    </row>
+    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="7">
-        <v>45856</v>
-      </c>
-      <c r="C9" s="8">
-        <v>45856</v>
+      <c r="B9" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>52</v>
       </c>
       <c r="D9" s="9">
         <v>24</v>
@@ -885,16 +999,18 @@
       <c r="H9" s="9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+    </row>
+    <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="7">
-        <v>45862</v>
-      </c>
-      <c r="C10" s="8">
-        <v>45862</v>
+      <c r="B10" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>53</v>
       </c>
       <c r="D10" s="9">
         <v>24</v>
@@ -911,16 +1027,18 @@
       <c r="H10" s="9" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+    </row>
+    <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="7">
-        <v>45867</v>
-      </c>
-      <c r="C11" s="13">
-        <v>45867</v>
+      <c r="B11" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>54</v>
       </c>
       <c r="D11" s="11">
         <v>24</v>
@@ -937,16 +1055,18 @@
       <c r="H11" s="11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+    </row>
+    <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="7">
-        <v>45867</v>
-      </c>
-      <c r="C12" s="8">
-        <v>45869</v>
+      <c r="B12" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>55</v>
       </c>
       <c r="D12" s="11">
         <v>37</v>
@@ -963,16 +1083,18 @@
       <c r="H12" s="11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+    </row>
+    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="7">
-        <v>45874</v>
-      </c>
-      <c r="C13" s="8">
-        <v>45874</v>
+      <c r="B13" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>56</v>
       </c>
       <c r="D13" s="9">
         <v>24</v>
@@ -989,16 +1111,18 @@
       <c r="H13" s="9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+    </row>
+    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="7">
-        <v>45881</v>
-      </c>
-      <c r="C14" s="8">
-        <v>45881</v>
+      <c r="B14" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>57</v>
       </c>
       <c r="D14" s="9">
         <v>24</v>
@@ -1015,16 +1139,18 @@
       <c r="H14" s="9" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+    </row>
+    <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="7">
-        <v>45880</v>
-      </c>
-      <c r="C15" s="8">
-        <v>45882</v>
+      <c r="B15" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>59</v>
       </c>
       <c r="D15" s="9">
         <v>39</v>
@@ -1041,16 +1167,18 @@
       <c r="H15" s="9" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+    </row>
+    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="7">
-        <v>45888</v>
-      </c>
-      <c r="C16" s="8">
-        <v>45888</v>
+      <c r="B16" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>60</v>
       </c>
       <c r="D16" s="9">
         <v>24</v>
@@ -1067,16 +1195,18 @@
       <c r="H16" s="9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+    </row>
+    <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="7">
-        <v>45895</v>
-      </c>
-      <c r="C17" s="8">
-        <v>45895</v>
+      <c r="B17" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>61</v>
       </c>
       <c r="D17" s="9">
         <v>24</v>
@@ -1093,16 +1223,18 @@
       <c r="H17" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+    </row>
+    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="7">
-        <v>45894</v>
-      </c>
-      <c r="C18" s="8">
-        <v>45897</v>
+      <c r="B18" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>63</v>
       </c>
       <c r="D18" s="9">
         <v>40</v>
@@ -1119,15 +1251,19 @@
       <c r="H18" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+    </row>
+    <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="7">
-        <v>45902</v>
-      </c>
-      <c r="C19" s="8"/>
+      <c r="B19" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>64</v>
+      </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9">
         <v>0</v>
@@ -1141,8 +1277,10 @@
       <c r="H19" s="9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+    </row>
+    <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>33</v>
       </c>
@@ -1156,15 +1294,17 @@
       <c r="G20" s="15"/>
       <c r="H20" s="16"/>
     </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="7">
-        <v>45909</v>
-      </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="9"/>
+      <c r="B21" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="18"/>
       <c r="E21" s="9">
         <v>0</v>
       </c>
@@ -1178,14 +1318,10 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="E22" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B20:H20"/>
+    <mergeCell ref="C21:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1194,28 +1330,281 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9DF1A92-06C4-4247-AAFB-D1D9EE5AD23D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8.88671875" style="24"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="19">
+        <v>45810</v>
+      </c>
+      <c r="B1" s="8">
+        <v>45812</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A2" s="19">
+        <v>45825</v>
+      </c>
+      <c r="B2" s="8">
+        <v>45826</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A3" s="19">
+        <v>45832</v>
+      </c>
+      <c r="B3" s="8">
+        <v>45832</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A4" s="19">
+        <v>45838</v>
+      </c>
+      <c r="B4" s="8">
+        <v>45840</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A5" s="19">
+        <v>45839</v>
+      </c>
+      <c r="B5" s="8">
+        <v>45839</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A6" s="19">
+        <v>45846</v>
+      </c>
+      <c r="B6" s="8">
+        <v>45846</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A7" s="19">
+        <v>45852</v>
+      </c>
+      <c r="B7" s="8">
+        <v>45854</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A8" s="19">
+        <v>45856</v>
+      </c>
+      <c r="B8" s="8">
+        <v>45856</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A9" s="19">
+        <v>45862</v>
+      </c>
+      <c r="B9" s="8">
+        <v>45862</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A10" s="19">
+        <v>45867</v>
+      </c>
+      <c r="B10" s="20">
+        <v>45867</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A11" s="19">
+        <v>45867</v>
+      </c>
+      <c r="B11" s="8">
+        <v>45869</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A12" s="19">
+        <v>45874</v>
+      </c>
+      <c r="B12" s="8">
+        <v>45874</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A13" s="19">
+        <v>45881</v>
+      </c>
+      <c r="B13" s="8">
+        <v>45881</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A14" s="19">
+        <v>45880</v>
+      </c>
+      <c r="B14" s="8">
+        <v>45882</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A15" s="19">
+        <v>45888</v>
+      </c>
+      <c r="B15" s="8">
+        <v>45888</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A16" s="19">
+        <v>45895</v>
+      </c>
+      <c r="B16" s="8">
+        <v>45895</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A17" s="19">
+        <v>45894</v>
+      </c>
+      <c r="B17" s="8">
+        <v>45897</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A18" s="19">
+        <v>45902</v>
+      </c>
+      <c r="B18" s="8">
+        <v>45902</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E19" s="24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E1862A7241CD5C4BB9A49AEC91EB145E" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="886e3144d6cee8faf22c18b9e81acb9a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="26e7f4b6-3714-4cf5-b0ae-a47b16f23eba" xmlns:ns4="c867d1a5-5827-4927-b797-91c0fe867b8f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c61be2c3ea34d5299ef19bcff063b94d" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1453,7 +1842,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -1463,15 +1852,16 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07190D35-2B79-4947-B2FC-84D221FCAD95}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96AA63C6-33C3-4EB8-B4D2-A24079D6B709}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1491,7 +1881,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB6D1C6B-FB84-4815-8B95-A837F1662AF0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -1507,4 +1897,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07190D35-2B79-4947-B2FC-84D221FCAD95}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>